<commit_message>
First part of fixes, before adding new content
</commit_message>
<xml_diff>
--- a/docs/Badania.xlsx
+++ b/docs/Badania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Projects/fuzzybase/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7B0B28-168C-AC44-946D-EEBA899A7E8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF975CA1-5E4B-E84E-A245-0904BA01CED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="3" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,12 @@
     <sheet name="Test 3" sheetId="3" r:id="rId3"/>
     <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Test 1'!$B$4:$B$23</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Test 1'!$B$4:$B$23</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Test 1'!$B$4:$B$23</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Test 1'!$B$4:$B$23</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Średnia</t>
   </si>
@@ -76,6 +82,18 @@
   </si>
   <si>
     <t>VDOM</t>
+  </si>
+  <si>
+    <t>IPC śr</t>
+  </si>
+  <si>
+    <t>IPC odch</t>
+  </si>
+  <si>
+    <t>SQL śr</t>
+  </si>
+  <si>
+    <t>SQL odch</t>
   </si>
 </sst>
 </file>
@@ -129,9 +147,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -143,6 +158,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -190,7 +208,7 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
-                <a:lumMod val="85000"/>
+                <a:lumMod val="65000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -358,10 +376,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>16.876929167291159</c:v>
+                    <c:v>33.753858334582318</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>14.076222218972486</c:v>
+                    <c:v>28.152444437944972</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -373,10 +391,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>16.876929167291159</c:v>
+                    <c:v>33.753858334582318</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>14.076222218972486</c:v>
+                    <c:v>28.152444437944972</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -439,7 +457,7 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="bg1">
-                <a:lumMod val="95000"/>
+                <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -518,10 +536,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>4.4398494592781672</c:v>
+                    <c:v>8.8796989185563344</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.8582781948196305</c:v>
+                    <c:v>3.716556389639261</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -533,10 +551,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>4.4398494592781672</c:v>
+                    <c:v>8.8796989185563344</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.8582781948196305</c:v>
+                    <c:v>3.716556389639261</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -987,10 +1005,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>440.21803123663392</c:v>
+                    <c:v>880.43606247326784</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3533340082965837</c:v>
+                    <c:v>4.7066680165931674</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1002,10 +1020,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>440.21803123663392</c:v>
+                    <c:v>880.43606247326784</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.3533340082965837</c:v>
+                    <c:v>4.7066680165931674</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1426,10 +1444,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>5.6382846119304402</c:v>
+                    <c:v>11.27656922386088</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>13.182089968969231</c:v>
+                    <c:v>26.364179937938463</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1441,10 +1459,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="0">
-                    <c:v>5.6382846119304402</c:v>
+                    <c:v>11.27656922386088</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>13.182089968969231</c:v>
+                    <c:v>26.364179937938463</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1762,12 +1780,10 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="x"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
@@ -1883,12 +1899,10 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="x"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
@@ -1897,6 +1911,124 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdDev"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$45:$L$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>1.4680814547887755</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7483329627982611</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.2589005243585558</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.0072237962970281</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.3478194002726824</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.8764012603470883</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.2183683345512368</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.1250115420035796</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>17.131918502577211</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>15.00666518584325</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>37.881914862955526</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$45:$L$45</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>1.4680814547887755</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.7483329627982611</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.2589005243585558</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.0072237962970281</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.3478194002726824</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.8764012603470883</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.2183683345512368</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.1250115420035796</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>17.131918502577211</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>15.00666518584325</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>37.881914862955526</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz4!$B$1:$L$1</c:f>
@@ -1941,7 +2073,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$45:$L$45</c:f>
+              <c:f>Arkusz4!$B$46:$L$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2007,15 +2139,10 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="x"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
@@ -2027,6 +2154,109 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$68:$L$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>1.2937094768634554</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2612081311339516</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3232237130876228</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.1001253095445223</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.5850567051229989</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.5128471582454699</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.9282996585956464</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>10.44836930112214</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>23.647576931619056</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>34.258921235358912</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>90.034657069842893</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$68:$L$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>1.2937094768634554</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.2612081311339516</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3232237130876228</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.1001253095445223</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3.5850567051229989</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.5128471582454699</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.9282996585956464</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>10.44836930112214</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>23.647576931619056</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>34.258921235358912</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>90.034657069842893</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Arkusz4!$B$1:$L$1</c:f>
@@ -2071,7 +2301,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$67:$L$67</c:f>
+              <c:f>Arkusz4!$B$69:$L$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2457,6 +2687,42 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{4F483CB9-F221-5A44-B7B6-E5F3C989CC7A}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="5"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2617,6 +2883,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3121,6 +3427,514 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3625,7 +4439,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4130,7 +4944,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4682,6 +5496,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>679172</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53008</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>13252</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Wykres 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38719965-3589-0845-8870-52AFFD62C3A9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5847520" y="5817704"/>
+              <a:ext cx="5626653" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pl-PL" sz="1100"/>
+                <a:t>Ten wykres jest niedostępny w Twojej wersji programu Excel.
+Edytowanie tego kształtu lub zapisanie tego skoroszytu w innym formacie pliku spowoduje trwałe uszkodzenie wykresu.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4781,10 +5673,10 @@
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>659236</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5111,8 +6003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEBF732-4E2E-8A43-9A69-0B0C7345129F}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5121,22 +6013,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5496,14 +6388,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -5531,20 +6423,20 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B4:B23)/2</f>
-        <v>16.876929167291159</v>
+        <f>STDEV(B4:B23)</f>
+        <v>33.753858334582318</v>
       </c>
       <c r="C28">
-        <f>STDEV(C4:C23)/2</f>
-        <v>4.4398494592781672</v>
+        <f t="shared" ref="C28:E28" si="0">STDEV(C4:C23)</f>
+        <v>8.8796989185563344</v>
       </c>
       <c r="D28">
-        <f>STDEV(D4:D23)/2</f>
-        <v>14.076222218972486</v>
+        <f t="shared" si="0"/>
+        <v>28.152444437944972</v>
       </c>
       <c r="E28">
-        <f>STDEV(E4:E23)/2</f>
-        <v>1.8582781948196305</v>
+        <f t="shared" si="0"/>
+        <v>3.716556389639261</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -5552,19 +6444,19 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <f>(2*B28)/B27</f>
+        <f>B28/B27</f>
         <v>9.1714104613540737E-2</v>
       </c>
       <c r="C29">
-        <f>(2*C28)/C27</f>
+        <f t="shared" ref="C29:E29" si="1">C28/C27</f>
         <v>5.8204481100969409E-2</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:E29" si="0">(2*D28)/D27</f>
+        <f t="shared" si="1"/>
         <v>7.871476090389963E-2</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1652448706404938E-2</v>
       </c>
     </row>
@@ -5596,7 +6488,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5605,8 +6497,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -5861,12 +6753,12 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B3:B22)/2</f>
-        <v>440.21803123663392</v>
+        <f>STDEV(B3:B22)</f>
+        <v>880.43606247326784</v>
       </c>
       <c r="C28">
-        <f>STDEV(C3:C22)/2</f>
-        <v>2.3533340082965837</v>
+        <f>STDEV(C3:C22)</f>
+        <v>4.7066680165931674</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -5874,11 +6766,11 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <f>(2*B28)/B27</f>
+        <f>B28/B27</f>
         <v>3.6966599671854991E-2</v>
       </c>
       <c r="C29">
-        <f>(2*C28)/C27</f>
+        <f>C28/C27</f>
         <v>3.5106533629300968E-2</v>
       </c>
     </row>
@@ -5901,8 +6793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F96CEA2-1E68-C84F-A146-EF1C68E3C1DA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5911,8 +6803,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6167,12 +7059,12 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B3:B22)/2</f>
-        <v>5.6382846119304402</v>
+        <f>STDEV(B3:B22)</f>
+        <v>11.27656922386088</v>
       </c>
       <c r="C28">
-        <f>STDEV(C3:C22)/2</f>
-        <v>13.182089968969231</v>
+        <f>STDEV(C3:C22)</f>
+        <v>26.364179937938463</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -6180,11 +7072,11 @@
         <v>10</v>
       </c>
       <c r="B29">
-        <f>(2*B28)/B27</f>
+        <f>(B28)/B27</f>
         <v>3.94159878145902E-2</v>
       </c>
       <c r="C29">
-        <f>(2*C28)/C27</f>
+        <f>(C28)/C27</f>
         <v>0.15973382686615969</v>
       </c>
     </row>
@@ -6205,10 +7097,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF00F0C-DDD1-EF4D-9C66-CBCF02B449F2}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView zoomScale="50" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6217,58 +7109,58 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>100</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>200</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>500</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>1000</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>2000</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>5000</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>10000</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>20000</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>50000</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>100000</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>200000</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="3"/>
       <c r="B3">
         <v>1</v>
       </c>
@@ -6304,7 +7196,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
       <c r="B4">
         <v>1</v>
       </c>
@@ -6340,7 +7232,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -6376,7 +7268,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="3"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -6412,7 +7304,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="3"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -6448,7 +7340,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="3"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -6484,7 +7376,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="3"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -6520,7 +7412,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -6556,7 +7448,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -6592,7 +7484,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -6628,7 +7520,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
       <c r="B13">
         <v>1</v>
       </c>
@@ -6664,7 +7556,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
       <c r="B14">
         <v>1</v>
       </c>
@@ -6700,7 +7592,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="3"/>
       <c r="B15">
         <v>1</v>
       </c>
@@ -6736,7 +7628,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="3"/>
       <c r="B16">
         <v>1</v>
       </c>
@@ -6772,7 +7664,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="3"/>
       <c r="B17">
         <v>1</v>
       </c>
@@ -6808,7 +7700,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -6844,7 +7736,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -6880,7 +7772,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
       <c r="B20">
         <v>1</v>
       </c>
@@ -6916,7 +7808,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
       <c r="B21">
         <v>1</v>
       </c>
@@ -6952,7 +7844,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
+      <c r="A22" s="3"/>
       <c r="B22">
         <v>1</v>
       </c>
@@ -6988,72 +7880,72 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <f>AVERAGE(B3:B22)</f>
         <v>1</v>
       </c>
-      <c r="C23" s="7">
-        <f t="shared" ref="C23:O23" si="0">AVERAGE(C3:C22)</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="6">
+        <f t="shared" ref="C23:L23" si="0">AVERAGE(C3:C22)</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3"/>
       <c r="B25">
         <v>13</v>
       </c>
@@ -7089,7 +7981,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3"/>
       <c r="B26">
         <v>13</v>
       </c>
@@ -7125,7 +8017,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
       <c r="B27">
         <v>11</v>
       </c>
@@ -7161,7 +8053,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3"/>
       <c r="B28">
         <v>11</v>
       </c>
@@ -7197,7 +8089,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" s="3"/>
       <c r="B29">
         <v>11</v>
       </c>
@@ -7233,7 +8125,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
+      <c r="A30" s="3"/>
       <c r="B30">
         <v>9</v>
       </c>
@@ -7269,7 +8161,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
       <c r="B31">
         <v>12</v>
       </c>
@@ -7305,7 +8197,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
       <c r="B32">
         <v>10</v>
       </c>
@@ -7341,7 +8233,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
       <c r="B33">
         <v>11</v>
       </c>
@@ -7377,7 +8269,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
       <c r="B34">
         <v>12</v>
       </c>
@@ -7413,7 +8305,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
+      <c r="A35" s="3"/>
       <c r="B35">
         <v>12</v>
       </c>
@@ -7449,7 +8341,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
+      <c r="A36" s="3"/>
       <c r="B36">
         <v>11</v>
       </c>
@@ -7485,7 +8377,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
+      <c r="A37" s="3"/>
       <c r="B37">
         <v>11</v>
       </c>
@@ -7521,7 +8413,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
+      <c r="A38" s="3"/>
       <c r="B38">
         <v>13</v>
       </c>
@@ -7557,7 +8449,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
+      <c r="A39" s="3"/>
       <c r="B39">
         <v>12</v>
       </c>
@@ -7593,7 +8485,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
+      <c r="A40" s="3"/>
       <c r="B40">
         <v>10</v>
       </c>
@@ -7629,7 +8521,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
+      <c r="A41" s="3"/>
       <c r="B41">
         <v>14</v>
       </c>
@@ -7665,7 +8557,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="4"/>
+      <c r="A42" s="3"/>
       <c r="B42">
         <v>10</v>
       </c>
@@ -7772,134 +8664,148 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="7">
+        <v>17</v>
+      </c>
+      <c r="B45">
+        <f>STDEV(B25:B44)</f>
+        <v>1.4680814547887755</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:L45" si="1">STDEV(C25:C44)</f>
+        <v>3.7483329627982611</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>2.2589005243585558</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>2.0072237962970281</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>3.3478194002726824</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>2.8764012603470883</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>3.2183683345512368</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>7.1250115420035796</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>17.131918502577211</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>15.00666518584325</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>37.881914862955526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="6">
         <f>AVERAGE(B25:B44)</f>
         <v>11.45</v>
       </c>
-      <c r="C45" s="7">
-        <f t="shared" ref="C45:O45" si="1">AVERAGE(C25:C44)</f>
+      <c r="C46" s="6">
+        <f t="shared" ref="C46:L46" si="2">AVERAGE(C25:C44)</f>
         <v>17.45</v>
       </c>
-      <c r="D45" s="7">
-        <f t="shared" si="1"/>
+      <c r="D46" s="6">
+        <f t="shared" si="2"/>
         <v>14.95</v>
       </c>
-      <c r="E45" s="7">
-        <f t="shared" si="1"/>
+      <c r="E46" s="6">
+        <f t="shared" si="2"/>
         <v>23.15</v>
       </c>
-      <c r="F45" s="7">
-        <f t="shared" si="1"/>
+      <c r="F46" s="6">
+        <f t="shared" si="2"/>
         <v>31.95</v>
       </c>
-      <c r="G45" s="7">
-        <f t="shared" si="1"/>
+      <c r="G46" s="6">
+        <f t="shared" si="2"/>
         <v>64.8</v>
       </c>
-      <c r="H45" s="7">
-        <f t="shared" si="1"/>
+      <c r="H46" s="6">
+        <f t="shared" si="2"/>
         <v>118.4</v>
       </c>
-      <c r="I45" s="7">
-        <f t="shared" si="1"/>
+      <c r="I46" s="6">
+        <f t="shared" si="2"/>
         <v>230.85</v>
       </c>
-      <c r="J45" s="7">
-        <f t="shared" si="1"/>
+      <c r="J46" s="6">
+        <f t="shared" si="2"/>
         <v>565.35</v>
       </c>
-      <c r="K45" s="7">
-        <f t="shared" si="1"/>
+      <c r="K46" s="6">
+        <f t="shared" si="2"/>
         <v>1140.4000000000001</v>
       </c>
-      <c r="L45" s="7">
-        <f t="shared" si="1"/>
+      <c r="L46" s="6">
+        <f t="shared" si="2"/>
         <v>2350.75</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B47">
-        <v>15</v>
-      </c>
-      <c r="C47">
-        <v>20</v>
-      </c>
-      <c r="D47">
-        <v>18</v>
-      </c>
-      <c r="E47">
-        <v>30</v>
-      </c>
-      <c r="F47">
-        <v>33</v>
-      </c>
-      <c r="G47">
-        <v>82</v>
-      </c>
-      <c r="H47">
-        <v>146</v>
-      </c>
-      <c r="I47">
-        <v>288</v>
-      </c>
-      <c r="J47">
-        <v>706</v>
-      </c>
-      <c r="K47">
-        <v>1473</v>
-      </c>
-      <c r="L47">
-        <v>3084</v>
-      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B48">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E48">
         <v>30</v>
       </c>
       <c r="F48">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G48">
         <v>82</v>
       </c>
       <c r="H48">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I48">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="J48">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="K48">
-        <v>1457</v>
+        <v>1473</v>
       </c>
       <c r="L48">
         <v>3084</v>
@@ -7910,19 +8816,19 @@
         <v>14</v>
       </c>
       <c r="C49">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D49">
         <v>20</v>
       </c>
       <c r="E49">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F49">
         <v>34</v>
       </c>
       <c r="G49">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H49">
         <v>154</v>
@@ -7931,48 +8837,48 @@
         <v>284</v>
       </c>
       <c r="J49">
-        <v>772</v>
+        <v>710</v>
       </c>
       <c r="K49">
-        <v>1476</v>
+        <v>1457</v>
       </c>
       <c r="L49">
-        <v>3020</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B50">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C50">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E50">
         <v>27</v>
       </c>
       <c r="F50">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G50">
         <v>81</v>
       </c>
       <c r="H50">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I50">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="J50">
-        <v>700</v>
+        <v>772</v>
       </c>
       <c r="K50">
-        <v>1536</v>
+        <v>1476</v>
       </c>
       <c r="L50">
-        <v>3084</v>
+        <v>3020</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
@@ -7980,19 +8886,19 @@
         <v>13</v>
       </c>
       <c r="C51">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E51">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F51">
         <v>39</v>
       </c>
       <c r="G51">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H51">
         <v>144</v>
@@ -8001,13 +8907,13 @@
         <v>290</v>
       </c>
       <c r="J51">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="K51">
-        <v>1414</v>
+        <v>1536</v>
       </c>
       <c r="L51">
-        <v>2884</v>
+        <v>3084</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
@@ -8015,34 +8921,34 @@
         <v>13</v>
       </c>
       <c r="C52">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>16</v>
       </c>
       <c r="E52">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F52">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G52">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H52">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="I52">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="J52">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="K52">
-        <v>1427</v>
+        <v>1414</v>
       </c>
       <c r="L52">
-        <v>3049</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
@@ -8056,16 +8962,16 @@
         <v>16</v>
       </c>
       <c r="E53">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F53">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G53">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H53">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="I53">
         <v>285</v>
@@ -8074,18 +8980,18 @@
         <v>700</v>
       </c>
       <c r="K53">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="L53">
-        <v>2892</v>
+        <v>3049</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B54">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C54">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D54">
         <v>16</v>
@@ -8094,7 +9000,7 @@
         <v>27</v>
       </c>
       <c r="F54">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G54">
         <v>85</v>
@@ -8103,16 +9009,16 @@
         <v>141</v>
       </c>
       <c r="I54">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="J54">
-        <v>742</v>
+        <v>700</v>
       </c>
       <c r="K54">
-        <v>1426</v>
+        <v>1429</v>
       </c>
       <c r="L54">
-        <v>3016</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
@@ -8123,7 +9029,7 @@
         <v>16</v>
       </c>
       <c r="D55">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E55">
         <v>27</v>
@@ -8132,30 +9038,30 @@
         <v>39</v>
       </c>
       <c r="G55">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H55">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I55">
         <v>307</v>
       </c>
       <c r="J55">
-        <v>705</v>
+        <v>742</v>
       </c>
       <c r="K55">
-        <v>1393</v>
+        <v>1426</v>
       </c>
       <c r="L55">
-        <v>2983</v>
+        <v>3016</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B56">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D56">
         <v>21</v>
@@ -8164,7 +9070,7 @@
         <v>27</v>
       </c>
       <c r="F56">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G56">
         <v>79</v>
@@ -8173,56 +9079,56 @@
         <v>146</v>
       </c>
       <c r="I56">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="J56">
         <v>705</v>
       </c>
       <c r="K56">
-        <v>1497</v>
+        <v>1393</v>
       </c>
       <c r="L56">
-        <v>2951</v>
+        <v>2983</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B57">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D57">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E57">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F57">
         <v>43</v>
       </c>
       <c r="G57">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H57">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I57">
         <v>284</v>
       </c>
       <c r="J57">
-        <v>748</v>
+        <v>705</v>
       </c>
       <c r="K57">
-        <v>1422</v>
+        <v>1497</v>
       </c>
       <c r="L57">
-        <v>2834</v>
+        <v>2951</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B58">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C58">
         <v>24</v>
@@ -8234,25 +9140,25 @@
         <v>26</v>
       </c>
       <c r="F58">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G58">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H58">
         <v>148</v>
       </c>
       <c r="I58">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="J58">
-        <v>687</v>
+        <v>748</v>
       </c>
       <c r="K58">
-        <v>1429</v>
+        <v>1422</v>
       </c>
       <c r="L58">
-        <v>2870</v>
+        <v>2834</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
@@ -8260,13 +9166,13 @@
         <v>12</v>
       </c>
       <c r="C59">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D59">
         <v>16</v>
       </c>
       <c r="E59">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F59">
         <v>37</v>
@@ -8275,54 +9181,54 @@
         <v>78</v>
       </c>
       <c r="H59">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I59">
         <v>275</v>
       </c>
       <c r="J59">
-        <v>753</v>
+        <v>687</v>
       </c>
       <c r="K59">
         <v>1429</v>
       </c>
       <c r="L59">
-        <v>3026</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B60">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C60">
         <v>21</v>
       </c>
       <c r="D60">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E60">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F60">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G60">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H60">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I60">
-        <v>302</v>
+        <v>275</v>
       </c>
       <c r="J60">
-        <v>685</v>
+        <v>753</v>
       </c>
       <c r="K60">
-        <v>1425</v>
+        <v>1429</v>
       </c>
       <c r="L60">
-        <v>3046</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
@@ -8330,7 +9236,7 @@
         <v>14</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D61">
         <v>15</v>
@@ -8342,7 +9248,7 @@
         <v>39</v>
       </c>
       <c r="G61">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H61">
         <v>150</v>
@@ -8351,68 +9257,68 @@
         <v>302</v>
       </c>
       <c r="J61">
-        <v>704</v>
+        <v>685</v>
       </c>
       <c r="K61">
-        <v>1386</v>
+        <v>1425</v>
       </c>
       <c r="L61">
-        <v>2936</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B62">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62">
         <v>15</v>
       </c>
       <c r="E62">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F62">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G62">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="H62">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="I62">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="J62">
-        <v>719</v>
+        <v>704</v>
       </c>
       <c r="K62">
-        <v>1444</v>
+        <v>1386</v>
       </c>
       <c r="L62">
-        <v>3078</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B63">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C63">
         <v>19</v>
       </c>
       <c r="D63">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E63">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F63">
         <v>45</v>
       </c>
       <c r="G63">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H63">
         <v>146</v>
@@ -8421,62 +9327,62 @@
         <v>301</v>
       </c>
       <c r="J63">
-        <v>703</v>
+        <v>719</v>
       </c>
       <c r="K63">
-        <v>1433</v>
+        <v>1444</v>
       </c>
       <c r="L63">
-        <v>2949</v>
+        <v>3078</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B64">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C64">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D64">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E64">
         <v>26</v>
       </c>
       <c r="F64">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G64">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H64">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="I64">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="J64">
-        <v>687</v>
+        <v>703</v>
       </c>
       <c r="K64">
-        <v>1445</v>
+        <v>1433</v>
       </c>
       <c r="L64">
-        <v>2869</v>
+        <v>2949</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B65">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E65">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F65">
         <v>40</v>
@@ -8485,24 +9391,24 @@
         <v>85</v>
       </c>
       <c r="H65">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I65">
         <v>284</v>
       </c>
       <c r="J65">
-        <v>713</v>
+        <v>687</v>
       </c>
       <c r="K65">
-        <v>1440</v>
+        <v>1445</v>
       </c>
       <c r="L65">
-        <v>3133</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B66">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C66">
         <v>20</v>
@@ -8511,76 +9417,160 @@
         <v>21</v>
       </c>
       <c r="E66">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F66">
         <v>40</v>
       </c>
       <c r="G66">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H66">
         <v>161</v>
       </c>
       <c r="I66">
+        <v>284</v>
+      </c>
+      <c r="J66">
+        <v>713</v>
+      </c>
+      <c r="K66">
+        <v>1440</v>
+      </c>
+      <c r="L66">
+        <v>3133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>15</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+      <c r="D67">
+        <v>21</v>
+      </c>
+      <c r="E67">
+        <v>23</v>
+      </c>
+      <c r="F67">
+        <v>40</v>
+      </c>
+      <c r="G67">
+        <v>93</v>
+      </c>
+      <c r="H67">
+        <v>161</v>
+      </c>
+      <c r="I67">
         <v>274</v>
       </c>
-      <c r="J66">
+      <c r="J67">
         <v>710</v>
       </c>
-      <c r="K66">
+      <c r="K67">
         <v>1437</v>
       </c>
-      <c r="L66">
+      <c r="L67">
         <v>2889</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="7">
-        <f>AVERAGE(B47:B66)</f>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68">
+        <f>STDEV(B48:B67)</f>
+        <v>1.2937094768634554</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:L68" si="3">STDEV(C48:C67)</f>
+        <v>4.2612081311339516</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>2.3232237130876228</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="3"/>
+        <v>2.1001253095445223</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>3.5850567051229989</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="3"/>
+        <v>4.5128471582454699</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="3"/>
+        <v>5.9282996585956464</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="3"/>
+        <v>10.44836930112214</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="3"/>
+        <v>23.647576931619056</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="3"/>
+        <v>34.258921235358912</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="3"/>
+        <v>90.034657069842893</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="6">
+        <f>AVERAGE(B48:B67)</f>
         <v>13.1</v>
       </c>
-      <c r="C67" s="7">
-        <f t="shared" ref="C67:O67" si="2">AVERAGE(C47:C66)</f>
+      <c r="C69" s="6">
+        <f t="shared" ref="C69:L69" si="4">AVERAGE(C48:C67)</f>
         <v>19.5</v>
       </c>
-      <c r="D67" s="7">
-        <f>AVERAGE(D47:D66)</f>
+      <c r="D69" s="6">
+        <f>AVERAGE(D48:D67)</f>
         <v>17.649999999999999</v>
       </c>
-      <c r="E67" s="7">
-        <f t="shared" si="2"/>
+      <c r="E69" s="6">
+        <f t="shared" si="4"/>
         <v>26.9</v>
       </c>
-      <c r="F67" s="7">
-        <f t="shared" si="2"/>
+      <c r="F69" s="6">
+        <f t="shared" si="4"/>
         <v>38.700000000000003</v>
       </c>
-      <c r="G67" s="7">
-        <f t="shared" si="2"/>
+      <c r="G69" s="6">
+        <f t="shared" si="4"/>
         <v>81.05</v>
       </c>
-      <c r="H67" s="7">
-        <f t="shared" si="2"/>
+      <c r="H69" s="6">
+        <f t="shared" si="4"/>
         <v>149.25</v>
       </c>
-      <c r="I67" s="7">
-        <f t="shared" si="2"/>
+      <c r="I69" s="6">
+        <f t="shared" si="4"/>
         <v>289.3</v>
       </c>
-      <c r="J67" s="7">
-        <f t="shared" si="2"/>
+      <c r="J69" s="6">
+        <f t="shared" si="4"/>
         <v>712.05</v>
       </c>
-      <c r="K67" s="7">
-        <f t="shared" si="2"/>
+      <c r="K69" s="6">
+        <f t="shared" si="4"/>
         <v>1440.9</v>
       </c>
-      <c r="L67" s="7">
-        <f t="shared" si="2"/>
+      <c r="L69" s="6">
+        <f t="shared" si="4"/>
         <v>2983.85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DOC: Project description Graphing utility
</commit_message>
<xml_diff>
--- a/docs/Badania.xlsx
+++ b/docs/Badania.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Projects/fuzzybase/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF975CA1-5E4B-E84E-A245-0904BA01CED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB058AEF-82C7-6A4E-9A9B-BBBE773DB8BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="2" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test 2" sheetId="2" r:id="rId2"/>
     <sheet name="Test 3" sheetId="3" r:id="rId3"/>
     <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
+    <sheet name="Arkusz1" sheetId="5" r:id="rId5"/>
+    <sheet name="Arkusz2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Test 1'!$B$4:$B$23</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Test 1'!$B$4:$B$23</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Test 1'!$B$4:$B$23</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Test 1'!$B$4:$B$23</definedName>
+    <definedName name="a_1" localSheetId="4">Arkusz1!$O$10:$AC$20</definedName>
+    <definedName name="a_1" localSheetId="5">Arkusz2!$A$1:$O$11</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,8 +37,55 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{4B267711-D746-204D-94C6-E140F47FDDEF}" name="a" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/krzysiekmiemiec/Desktop/a.csv" decimal="," thousands=" " delimiter="|">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{7A4617BA-F144-2D40-83E6-488CE4414607}" name="a1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/krzysiekmiemiec/Desktop/a.csv" decimal="," thousands=" " delimiter="|">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
   <si>
     <t>Średnia</t>
   </si>
@@ -95,18 +146,125 @@
   <si>
     <t>SQL odch</t>
   </si>
+  <si>
+    <t xml:space="preserve"> t   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0.6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> age </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sex </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cp </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> trestbps </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chol </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fbs </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> restecg </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thalach </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exang </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oldpeak </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> slope </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ca </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thal </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> num </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    source     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> switzerland   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0.0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cleveland     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hungary       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> long_beach_va </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     2.2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1.0 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -142,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -5704,6 +5863,14 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="a_1" connectionId="1" xr16:uid="{25C4F06C-7F87-384E-B88E-2E0EEA3B1242}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="a_1" connectionId="2" xr16:uid="{9DE8B36B-9E72-0B41-8A24-D076A9C8DAD2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
@@ -6003,8 +6170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEBF732-4E2E-8A43-9A69-0B0C7345129F}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A5" zoomScale="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6423,11 +6590,11 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B4:B23)</f>
+        <f>STDEVA(B4:B23)</f>
         <v>33.753858334582318</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:E28" si="0">STDEV(C4:C23)</f>
+        <f t="shared" ref="C28:E28" si="0">STDEVA(C4:C23)</f>
         <v>8.8796989185563344</v>
       </c>
       <c r="D28">
@@ -6488,7 +6655,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C29"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6753,11 +6920,11 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B3:B22)</f>
+        <f>STDEVA(B3:B22)</f>
         <v>880.43606247326784</v>
       </c>
       <c r="C28">
-        <f>STDEV(C3:C22)</f>
+        <f>STDEVA(C3:C22)</f>
         <v>4.7066680165931674</v>
       </c>
     </row>
@@ -6793,8 +6960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F96CEA2-1E68-C84F-A146-EF1C68E3C1DA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7059,11 +7226,11 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>STDEV(B3:B22)</f>
+        <f>STDEVA(B3:B22)</f>
         <v>11.27656922386088</v>
       </c>
       <c r="C28">
-        <f>STDEV(C3:C22)</f>
+        <f>STDEVA(C3:C22)</f>
         <v>26.364179937938463</v>
       </c>
     </row>
@@ -9578,4 +9745,1110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22423169-F610-5D44-A197-3E9349A36209}">
+  <dimension ref="O10:AC20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O10" sqref="O10:AC20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" t="s">
+        <v>30</v>
+      </c>
+      <c r="V10" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" t="s">
+        <v>32</v>
+      </c>
+      <c r="X10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <v>60</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>130</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>41</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>130</v>
+      </c>
+      <c r="X11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11">
+        <v>3</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12">
+        <v>51</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>110</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>41</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>92</v>
+      </c>
+      <c r="X12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z12">
+        <v>2</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13">
+        <v>67</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>106</v>
+      </c>
+      <c r="T13">
+        <v>223</v>
+      </c>
+      <c r="U13" t="s">
+        <v>22</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>142</v>
+      </c>
+      <c r="X13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>2</v>
+      </c>
+      <c r="AB13">
+        <v>3</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
+        <v>48</v>
+      </c>
+      <c r="P14">
+        <v>35</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>120</v>
+      </c>
+      <c r="T14">
+        <v>160</v>
+      </c>
+      <c r="U14" t="s">
+        <v>22</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>185</v>
+      </c>
+      <c r="X14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O15" t="s">
+        <v>50</v>
+      </c>
+      <c r="P15">
+        <v>55</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <v>150</v>
+      </c>
+      <c r="T15">
+        <v>160</v>
+      </c>
+      <c r="U15" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>150</v>
+      </c>
+      <c r="X15" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O16" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16">
+        <v>56</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <v>130</v>
+      </c>
+      <c r="T16">
+        <v>256</v>
+      </c>
+      <c r="U16" t="s">
+        <v>20</v>
+      </c>
+      <c r="V16">
+        <v>2</v>
+      </c>
+      <c r="W16">
+        <v>142</v>
+      </c>
+      <c r="X16" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z16">
+        <v>2</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>6</v>
+      </c>
+      <c r="AC16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17">
+        <v>51</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>95</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>126</v>
+      </c>
+      <c r="X17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z17">
+        <v>2</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O18" t="s">
+        <v>48</v>
+      </c>
+      <c r="P18">
+        <v>46</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <v>118</v>
+      </c>
+      <c r="T18">
+        <v>186</v>
+      </c>
+      <c r="U18" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>124</v>
+      </c>
+      <c r="X18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB18">
+        <v>7</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19">
+        <v>65</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
+      <c r="S19">
+        <v>150</v>
+      </c>
+      <c r="T19">
+        <v>225</v>
+      </c>
+      <c r="U19" t="s">
+        <v>22</v>
+      </c>
+      <c r="V19">
+        <v>2</v>
+      </c>
+      <c r="W19">
+        <v>114</v>
+      </c>
+      <c r="X19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z19">
+        <v>2</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+      <c r="AB19">
+        <v>7</v>
+      </c>
+      <c r="AC19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="15:29" x14ac:dyDescent="0.2">
+      <c r="O20" t="s">
+        <v>48</v>
+      </c>
+      <c r="P20">
+        <v>50</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+      <c r="S20">
+        <v>145</v>
+      </c>
+      <c r="T20">
+        <v>264</v>
+      </c>
+      <c r="U20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>150</v>
+      </c>
+      <c r="X20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D14BEF-BBB9-6443-981F-D40A2FE47238}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>130</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>130</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>92</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>106</v>
+      </c>
+      <c r="F4">
+        <v>223</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>142</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>120</v>
+      </c>
+      <c r="F5">
+        <v>160</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>185</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+      <c r="F6">
+        <v>160</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>150</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>130</v>
+      </c>
+      <c r="F7">
+        <v>256</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>142</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>95</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>126</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>186</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>124</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>225</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>114</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>145</v>
+      </c>
+      <c r="F11">
+        <v>264</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>150</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" t="s">
+        <v>45</v>
+      </c>
+      <c r="N11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DOC: Improved chapters about fuzzy logic, research and project, added schematics Updated ResultsDOM component
</commit_message>
<xml_diff>
--- a/docs/Badania.xlsx
+++ b/docs/Badania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Projects/fuzzybase/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB058AEF-82C7-6A4E-9A9B-BBBE773DB8BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B545089C-0CCC-7B4C-9EA6-CBB718A021F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="2" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="3" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Test 1'!$B$4:$B$23</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Test 1'!$B$4:$B$23</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Test 1'!$B$4:$B$23</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Test 1'!$B$4:$B$23</definedName>
     <definedName name="a_1" localSheetId="4">Arkusz1!$O$10:$AC$20</definedName>
     <definedName name="a_1" localSheetId="5">Arkusz2!$A$1:$O$11</definedName>
   </definedNames>
@@ -85,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="58">
   <si>
     <t>Średnia</t>
   </si>
@@ -245,6 +242,21 @@
   <si>
     <t xml:space="preserve">     1.0 </t>
   </si>
+  <si>
+    <t>DOM</t>
+  </si>
+  <si>
+    <t>DOM odch</t>
+  </si>
+  <si>
+    <t>DOM śr</t>
+  </si>
+  <si>
+    <t>SUMA VDOM</t>
+  </si>
+  <si>
+    <t>SUMA DOM</t>
+  </si>
 </sst>
 </file>
 
@@ -316,10 +328,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2507,6 +2519,201 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>DOM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$91:$I$91</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.88704120832301658</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.9014167467189327</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.0981015164773336</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>26.084629472868539</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>105.66710387866804</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>153.30616082652526</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>327.11882196567433</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1308.4752878626973</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Arkusz4!$B$91:$I$91</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.88704120832301658</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.9014167467189327</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.0981015164773336</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>26.084629472868539</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>105.66710387866804</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>153.30616082652526</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>327.11882196567433</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1308.4752878626973</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$92:$L$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>233.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>453.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>873.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2272.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4566.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9D77-EE44-B39E-DDA86F745A26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2523,6 +2730,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2645,6 +2853,7 @@
         <c:axId val="1079410399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="8000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2760,6 +2969,592 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1079795807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Suma DOM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$95:$L$95</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>29.099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>265.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>503.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>943.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2418.4499999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4833.8999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18785.150000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6C9-B640-9078-E35DD1597F0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Suma VDOM</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz4!$B$94:$L$94</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>25.549999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.650000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>146.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>268.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>521.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1278.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2582.3000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5335.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D6C9-B640-9078-E35DD1597F0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="802124256"/>
+        <c:axId val="802125936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="802124256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba wierszy w wynikach zapytania</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802125936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25000"/>
+        <c:minorUnit val="10000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="802125936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Łączny</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> czas wykonania [ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802124256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3082,6 +3877,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5104,6 +5939,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5704,8 +7055,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5847520" y="5817704"/>
-              <a:ext cx="5626653" cy="2743200"/>
+              <a:off x="5835372" y="5945808"/>
+              <a:ext cx="5607327" cy="2805044"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5832,8 +7183,8 @@
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>659236</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>445954</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>19390</xdr:rowOff>
     </xdr:to>
@@ -5855,6 +7206,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360820</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>103822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>794474</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>7791</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E92B0C-7D7E-394C-B0C0-20B2F9537145}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6180,22 +7567,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -6555,14 +7942,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -6664,8 +8051,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6960,7 +8347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F96CEA2-1E68-C84F-A146-EF1C68E3C1DA}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -6970,8 +8357,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -7264,10 +8651,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF00F0C-DDD1-EF4D-9C66-CBCF02B449F2}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView tabSelected="1" topLeftCell="I56" zoomScale="116" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9739,6 +11126,722 @@
       <c r="L69" s="6">
         <f t="shared" si="4"/>
         <v>2983.85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71">
+        <v>55</v>
+      </c>
+      <c r="D71">
+        <v>226</v>
+      </c>
+      <c r="E71">
+        <v>471</v>
+      </c>
+      <c r="F71">
+        <v>533</v>
+      </c>
+      <c r="G71">
+        <v>2341</v>
+      </c>
+      <c r="H71">
+        <v>5001</v>
+      </c>
+      <c r="I71">
+        <f>4*H71</f>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <v>60</v>
+      </c>
+      <c r="D72">
+        <v>225</v>
+      </c>
+      <c r="E72">
+        <v>421</v>
+      </c>
+      <c r="F72">
+        <v>1080</v>
+      </c>
+      <c r="G72">
+        <v>2341</v>
+      </c>
+      <c r="H72">
+        <v>5001</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:I81" si="5">4*H72</f>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>63</v>
+      </c>
+      <c r="D73">
+        <v>225</v>
+      </c>
+      <c r="E73">
+        <v>421</v>
+      </c>
+      <c r="F73">
+        <v>1080</v>
+      </c>
+      <c r="G73">
+        <v>2199</v>
+      </c>
+      <c r="H73">
+        <v>4249</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="5"/>
+        <v>16996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>63</v>
+      </c>
+      <c r="D74">
+        <v>231</v>
+      </c>
+      <c r="E74">
+        <v>429</v>
+      </c>
+      <c r="F74">
+        <v>890</v>
+      </c>
+      <c r="G74">
+        <v>2199</v>
+      </c>
+      <c r="H74">
+        <v>4461</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="5"/>
+        <v>17844</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>61</v>
+      </c>
+      <c r="D75">
+        <v>223</v>
+      </c>
+      <c r="E75">
+        <v>429</v>
+      </c>
+      <c r="F75">
+        <v>890</v>
+      </c>
+      <c r="G75">
+        <v>2423</v>
+      </c>
+      <c r="H75">
+        <v>4351</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="5"/>
+        <v>17404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>62</v>
+      </c>
+      <c r="D76">
+        <v>226</v>
+      </c>
+      <c r="E76">
+        <v>447</v>
+      </c>
+      <c r="F76">
+        <v>866</v>
+      </c>
+      <c r="G76">
+        <v>2423</v>
+      </c>
+      <c r="H76">
+        <v>4218</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="5"/>
+        <v>16872</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>53</v>
+      </c>
+      <c r="D77">
+        <v>226</v>
+      </c>
+      <c r="E77">
+        <v>447</v>
+      </c>
+      <c r="F77">
+        <v>866</v>
+      </c>
+      <c r="G77">
+        <v>2067</v>
+      </c>
+      <c r="H77">
+        <v>4741</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="5"/>
+        <v>18964</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78">
+        <v>54</v>
+      </c>
+      <c r="D78">
+        <v>234</v>
+      </c>
+      <c r="E78">
+        <v>452</v>
+      </c>
+      <c r="F78">
+        <v>866</v>
+      </c>
+      <c r="G78">
+        <v>2067</v>
+      </c>
+      <c r="H78">
+        <v>5001</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="5"/>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <v>53</v>
+      </c>
+      <c r="D79">
+        <v>234</v>
+      </c>
+      <c r="E79">
+        <v>452</v>
+      </c>
+      <c r="F79">
+        <v>920</v>
+      </c>
+      <c r="G79">
+        <v>2512</v>
+      </c>
+      <c r="H79">
+        <v>5001</v>
+      </c>
+      <c r="I79">
+        <f>4*H79</f>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>3</v>
+      </c>
+      <c r="C80">
+        <v>52</v>
+      </c>
+      <c r="D80">
+        <v>237</v>
+      </c>
+      <c r="E80">
+        <v>501</v>
+      </c>
+      <c r="F80">
+        <v>884</v>
+      </c>
+      <c r="G80">
+        <v>2512</v>
+      </c>
+      <c r="H80">
+        <v>4249</v>
+      </c>
+      <c r="I80">
+        <f>4*H80</f>
+        <v>16996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>52</v>
+      </c>
+      <c r="D81">
+        <v>237</v>
+      </c>
+      <c r="E81">
+        <v>501</v>
+      </c>
+      <c r="F81">
+        <v>884</v>
+      </c>
+      <c r="G81">
+        <v>2096</v>
+      </c>
+      <c r="H81">
+        <v>4461</v>
+      </c>
+      <c r="I81">
+        <f t="shared" ref="I81:I90" si="6">4*H81</f>
+        <v>17844</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82">
+        <v>55</v>
+      </c>
+      <c r="D82">
+        <v>235</v>
+      </c>
+      <c r="E82">
+        <v>452</v>
+      </c>
+      <c r="F82">
+        <v>887</v>
+      </c>
+      <c r="G82">
+        <v>2096</v>
+      </c>
+      <c r="H82">
+        <v>4351</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="6"/>
+        <v>17404</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>4</v>
+      </c>
+      <c r="C83">
+        <v>53</v>
+      </c>
+      <c r="D83">
+        <v>235</v>
+      </c>
+      <c r="E83">
+        <v>452</v>
+      </c>
+      <c r="F83">
+        <v>887</v>
+      </c>
+      <c r="G83">
+        <v>2255</v>
+      </c>
+      <c r="H83">
+        <v>4218</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="6"/>
+        <v>16872</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>4</v>
+      </c>
+      <c r="C84">
+        <v>53</v>
+      </c>
+      <c r="D84">
+        <v>239</v>
+      </c>
+      <c r="E84">
+        <v>447</v>
+      </c>
+      <c r="F84">
+        <v>861</v>
+      </c>
+      <c r="G84">
+        <v>2255</v>
+      </c>
+      <c r="H84">
+        <v>4741</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="6"/>
+        <v>18964</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <v>53</v>
+      </c>
+      <c r="D85">
+        <v>239</v>
+      </c>
+      <c r="E85">
+        <v>447</v>
+      </c>
+      <c r="F85">
+        <v>861</v>
+      </c>
+      <c r="G85">
+        <v>2367</v>
+      </c>
+      <c r="H85">
+        <v>5001</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="6"/>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>4</v>
+      </c>
+      <c r="C86">
+        <v>58</v>
+      </c>
+      <c r="D86">
+        <v>242</v>
+      </c>
+      <c r="E86">
+        <v>447</v>
+      </c>
+      <c r="F86">
+        <v>845</v>
+      </c>
+      <c r="G86">
+        <v>2367</v>
+      </c>
+      <c r="H86">
+        <v>5001</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="6"/>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>4</v>
+      </c>
+      <c r="C87">
+        <v>58</v>
+      </c>
+      <c r="D87">
+        <v>242</v>
+      </c>
+      <c r="E87">
+        <v>447</v>
+      </c>
+      <c r="F87">
+        <v>845</v>
+      </c>
+      <c r="G87">
+        <v>2387</v>
+      </c>
+      <c r="H87">
+        <v>4249</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="6"/>
+        <v>16996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88">
+        <v>60</v>
+      </c>
+      <c r="D88">
+        <v>236</v>
+      </c>
+      <c r="E88">
+        <v>446</v>
+      </c>
+      <c r="F88">
+        <v>821</v>
+      </c>
+      <c r="G88">
+        <v>2387</v>
+      </c>
+      <c r="H88">
+        <v>4461</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="6"/>
+        <v>17844</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>60</v>
+      </c>
+      <c r="D89">
+        <v>236</v>
+      </c>
+      <c r="E89">
+        <v>446</v>
+      </c>
+      <c r="F89">
+        <v>821</v>
+      </c>
+      <c r="G89">
+        <v>2079</v>
+      </c>
+      <c r="H89">
+        <v>4351</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="6"/>
+        <v>17404</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>58</v>
+      </c>
+      <c r="D90">
+        <v>239</v>
+      </c>
+      <c r="E90">
+        <v>520</v>
+      </c>
+      <c r="F90">
+        <v>877</v>
+      </c>
+      <c r="G90">
+        <v>2079</v>
+      </c>
+      <c r="H90">
+        <v>4218</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="6"/>
+        <v>16872</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>54</v>
+      </c>
+      <c r="B91">
+        <f>STDEVA(B71:B90)</f>
+        <v>0.88704120832301658</v>
+      </c>
+      <c r="C91">
+        <f t="shared" ref="C91:L91" si="7">STDEVA(C71:C90)</f>
+        <v>3.9014167467189327</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="7"/>
+        <v>6.0981015164773336</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="7"/>
+        <v>26.084629472868539</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="7"/>
+        <v>105.66710387866804</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="7"/>
+        <v>153.30616082652526</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="7"/>
+        <v>327.11882196567433</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="7"/>
+        <v>1308.4752878626973</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92">
+        <f>AVERAGE(B71:B90)</f>
+        <v>4.55</v>
+      </c>
+      <c r="C92">
+        <f>AVERAGE(C71:C90)</f>
+        <v>56.8</v>
+      </c>
+      <c r="D92">
+        <f>AVERAGE(D71:D90)</f>
+        <v>233.35</v>
+      </c>
+      <c r="E92">
+        <f>AVERAGE(E71:E90)</f>
+        <v>453.75</v>
+      </c>
+      <c r="F92">
+        <f>AVERAGE(F71:F90)</f>
+        <v>873.2</v>
+      </c>
+      <c r="G92">
+        <f t="shared" ref="G92:H92" si="8">AVERAGE(G71:G90)</f>
+        <v>2272.6</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="8"/>
+        <v>4566.25</v>
+      </c>
+      <c r="I92">
+        <f>AVERAGE(I71:I90)</f>
+        <v>18265</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94">
+        <f>B23+B46+B69</f>
+        <v>25.549999999999997</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:L94" si="9">C23+C46+C69</f>
+        <v>37.950000000000003</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="9"/>
+        <v>33.599999999999994</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="9"/>
+        <v>51.05</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="9"/>
+        <v>71.650000000000006</v>
+      </c>
+      <c r="G94">
+        <f t="shared" si="9"/>
+        <v>146.85</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="9"/>
+        <v>268.64999999999998</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="9"/>
+        <v>521.15</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="9"/>
+        <v>1278.4000000000001</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="9"/>
+        <v>2582.3000000000002</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="9"/>
+        <v>5335.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>57</v>
+      </c>
+      <c r="B95">
+        <f>B69+B46+B92</f>
+        <v>29.099999999999998</v>
+      </c>
+      <c r="C95">
+        <f t="shared" ref="C95:L95" si="10">C69+C46+C92</f>
+        <v>93.75</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="10"/>
+        <v>265.95</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="10"/>
+        <v>503.8</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="10"/>
+        <v>943.85</v>
+      </c>
+      <c r="G95">
+        <f t="shared" si="10"/>
+        <v>2418.4499999999998</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="10"/>
+        <v>4833.8999999999996</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="10"/>
+        <v>18785.150000000001</v>
       </c>
     </row>
   </sheetData>
@@ -10331,50 +12434,50 @@
     <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Charts DOC: Updated and formatted files
</commit_message>
<xml_diff>
--- a/docs/Badania.xlsx
+++ b/docs/Badania.xlsx
@@ -8,22 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Projects/fuzzybase/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B545089C-0CCC-7B4C-9EA6-CBB718A021F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5461BAD-9EEA-F64E-B0D8-0995DFC5AC6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="3" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32100" windowHeight="19440" activeTab="4" xr2:uid="{F8583B78-D113-714E-A396-4A431EDAC67B}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test 2" sheetId="2" r:id="rId2"/>
     <sheet name="Test 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
-    <sheet name="Arkusz1" sheetId="5" r:id="rId5"/>
-    <sheet name="Arkusz2" sheetId="6" r:id="rId6"/>
+    <sheet name="Testy aplikacji" sheetId="4" r:id="rId4"/>
+    <sheet name="Arkusz1" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Test 1'!$B$4:$B$23</definedName>
-    <definedName name="a_1" localSheetId="4">Arkusz1!$O$10:$AC$20</definedName>
-    <definedName name="a_1" localSheetId="5">Arkusz2!$A$1:$O$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Arkusz1!$A$4:$A$14</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Arkusz1!$G$4:$G$14</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Arkusz1!$D$3</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Arkusz1!$D$4:$D$14</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Arkusz1!$G$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Arkusz1!$G$4:$G$14</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Arkusz1!$A$4:$A$14</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Arkusz1!$D$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Arkusz1!$D$4:$D$14</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Arkusz1!$G$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,55 +41,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{4B267711-D746-204D-94C6-E140F47FDDEF}" name="a" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr sourceFile="/Users/krzysiekmiemiec/Desktop/a.csv" decimal="," thousands=" " delimiter="|">
-      <textFields count="15">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" xr16:uid="{7A4617BA-F144-2D40-83E6-488CE4414607}" name="a1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr sourceFile="/Users/krzysiekmiemiec/Desktop/a.csv" decimal="," thousands=" " delimiter="|">
-      <textFields count="15">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Średnia</t>
   </si>
@@ -144,105 +104,6 @@
     <t>SQL odch</t>
   </si>
   <si>
-    <t xml:space="preserve"> t   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> f     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> f   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> t     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     0.6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> age </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sex </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cp </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> trestbps </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chol </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fbs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> restecg </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> thalach </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> exang </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> oldpeak </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> slope </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ca </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> thal </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> num </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    source     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> switzerland   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     1.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     0.0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cleveland     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     0.3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hungary       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> long_beach_va </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     2.2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     1.0 </t>
-  </si>
-  <si>
     <t>DOM</t>
   </si>
   <si>
@@ -257,26 +118,42 @@
   <si>
     <t>SUMA DOM</t>
   </si>
+  <si>
+    <t>ODCH DOM</t>
+  </si>
+  <si>
+    <t>ODCH VDOM</t>
+  </si>
+  <si>
+    <t>Zapytanie 3 (ostre)</t>
+  </si>
+  <si>
+    <t>Zapytanie 3 (rozmyte)</t>
+  </si>
+  <si>
+    <t>Zapytanie 2 (ostre)</t>
+  </si>
+  <si>
+    <t>Zapytanie 2 (rozmyte)</t>
+  </si>
+  <si>
+    <t>Zapytanie 1 (ostre)</t>
+  </si>
+  <si>
+    <t>Zapytanie 1 (rozmyte)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -312,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,10 +205,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1965,7 +1845,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2007,7 +1887,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$23:$L$23</c:f>
+              <c:f>'Testy aplikacji'!$B$23:$L$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2104,7 +1984,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Arkusz4!$B$45:$L$45</c:f>
+                <c:f>'Testy aplikacji'!$B$45:$L$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="11"/>
@@ -2146,7 +2026,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Arkusz4!$B$45:$L$45</c:f>
+                <c:f>'Testy aplikacji'!$B$45:$L$45</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="11"/>
@@ -2202,7 +2082,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2244,7 +2124,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$46:$L$46</c:f>
+              <c:f>'Testy aplikacji'!$B$46:$L$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2332,7 +2212,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Arkusz4!$B$68:$L$68</c:f>
+                <c:f>'Testy aplikacji'!$B$68:$L$68</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="11"/>
@@ -2374,7 +2254,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Arkusz4!$B$68:$L$68</c:f>
+                <c:f>'Testy aplikacji'!$B$68:$L$68</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="11"/>
@@ -2430,7 +2310,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2472,7 +2352,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$69:$L$69</c:f>
+              <c:f>'Testy aplikacji'!$B$69:$L$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2554,7 +2434,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Arkusz4!$B$91:$I$91</c:f>
+                <c:f>'Testy aplikacji'!$B$91:$I$91</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
@@ -2587,7 +2467,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Arkusz4!$B$91:$I$91</c:f>
+                <c:f>'Testy aplikacji'!$B$91:$I$91</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="8"/>
@@ -2634,7 +2514,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2676,7 +2556,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$92:$L$92</c:f>
+              <c:f>'Testy aplikacji'!$B$92:$L$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3079,7 +2959,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Suma DOM</c:v>
+            <c:v>DOM</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="9525" cap="rnd">
@@ -3103,9 +2983,94 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Testy aplikacji'!$B$98:$I$98</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>3.648832139975247</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11.910957840651147</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10.680225753923512</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>30.191978578710092</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>112.59997998406372</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>160.69540924511782</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>336.26548995882121</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1326.048668705823</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Testy aplikacji'!$B$98:$I$98</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>3.648832139975247</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11.910957840651147</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10.680225753923512</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>30.191978578710092</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>112.59997998406372</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>160.69540924511782</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>336.26548995882121</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1326.048668705823</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3147,9 +3112,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$95:$L$95</c:f>
+              <c:f>'Testy aplikacji'!$B$95:$L$95</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>29.099999999999998</c:v>
@@ -3189,7 +3154,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Suma VDOM</c:v>
+            <c:v>VDOM</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="9525" cap="rnd">
@@ -3213,9 +3178,112 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Testy aplikacji'!$B$97:$L$97</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>2.7617909316522309</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.0095410939322136</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.5821242374461786</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.1073491058415499</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.9328761053956818</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.3892484185925582</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.1466679931468828</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>17.573380843125719</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>40.779495434196264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>49.265586421202158</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>127.91657193279842</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Testy aplikacji'!$B$97:$L$97</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="11"/>
+                  <c:pt idx="0">
+                    <c:v>2.7617909316522309</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.0095410939322136</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.5821242374461786</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.1073491058415499</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.9328761053956818</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.3892484185925582</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.1466679931468828</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>17.573380843125719</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>40.779495434196264</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>49.265586421202158</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>127.91657193279842</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$1:$L$1</c:f>
+              <c:f>'Testy aplikacji'!$B$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3257,9 +3325,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz4!$B$94:$L$94</c:f>
+              <c:f>'Testy aplikacji'!$B$94:$L$94</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>25.549999999999997</c:v>
@@ -3517,7 +3585,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3568,6 +3636,1101 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 1 (ostre)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>311</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 2 (ostre)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>183</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 3 (ostre)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$D$4:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>124</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 1 (rozmyte)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$E$4:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>311</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 2 (rozmyte)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$F$4:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>139</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zapytanie 3 (rozmyte)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$G$4:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-06FC-E74A-B0E1-6EE4362A369A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="799288688"/>
+        <c:axId val="843024528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="799288688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Minimalny</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>topień przynależności</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="843024528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="843024528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba zwróconych wierszy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="799288688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3917,6 +5080,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6455,6 +7658,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7250,12 +8969,45 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="a_1" connectionId="1" xr16:uid="{25C4F06C-7F87-384E-B88E-2E0EEA3B1242}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="a_1" connectionId="2" xr16:uid="{9DE8B36B-9E72-0B41-8A24-D076A9C8DAD2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>248242</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>83616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>758692</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>185879</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{105FA4DF-0A3E-924A-92C5-61B4DFDC5EEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8651,10 +10403,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF00F0C-DDD1-EF4D-9C66-CBCF02B449F2}">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I56" zoomScale="116" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94:L95"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="I95" sqref="B95:I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11130,7 +12882,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -11194,7 +12946,7 @@
         <v>5001</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I81" si="5">4*H72</f>
+        <f t="shared" ref="I72:I78" si="5">4*H72</f>
         <v>20004</v>
       </c>
     </row>
@@ -11686,14 +13438,14 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B91">
         <f>STDEVA(B71:B90)</f>
         <v>0.88704120832301658</v>
       </c>
       <c r="C91">
-        <f t="shared" ref="C91:L91" si="7">STDEVA(C71:C90)</f>
+        <f t="shared" ref="C91:I91" si="7">STDEVA(C71:C90)</f>
         <v>3.9014167467189327</v>
       </c>
       <c r="D91">
@@ -11723,7 +13475,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B92">
         <f>AVERAGE(B71:B90)</f>
@@ -11760,88 +13512,174 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>56</v>
-      </c>
-      <c r="B94">
+        <v>23</v>
+      </c>
+      <c r="B94" s="9">
         <f>B23+B46+B69</f>
         <v>25.549999999999997</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="9">
         <f t="shared" ref="C94:L94" si="9">C23+C46+C69</f>
         <v>37.950000000000003</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="9">
         <f t="shared" si="9"/>
         <v>33.599999999999994</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="9">
         <f t="shared" si="9"/>
         <v>51.05</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="9">
         <f t="shared" si="9"/>
         <v>71.650000000000006</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="9">
         <f t="shared" si="9"/>
         <v>146.85</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="9">
         <f t="shared" si="9"/>
         <v>268.64999999999998</v>
       </c>
-      <c r="I94">
+      <c r="I94" s="9">
         <f t="shared" si="9"/>
         <v>521.15</v>
       </c>
-      <c r="J94">
+      <c r="J94" s="9">
         <f t="shared" si="9"/>
         <v>1278.4000000000001</v>
       </c>
-      <c r="K94">
+      <c r="K94" s="9">
         <f t="shared" si="9"/>
         <v>2582.3000000000002</v>
       </c>
-      <c r="L94">
+      <c r="L94" s="9">
         <f t="shared" si="9"/>
         <v>5335.6</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>57</v>
-      </c>
-      <c r="B95">
+        <v>24</v>
+      </c>
+      <c r="B95" s="9">
         <f>B69+B46+B92</f>
         <v>29.099999999999998</v>
       </c>
-      <c r="C95">
-        <f t="shared" ref="C95:L95" si="10">C69+C46+C92</f>
+      <c r="C95" s="9">
+        <f t="shared" ref="C95:I95" si="10">C69+C46+C92</f>
         <v>93.75</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="9">
         <f t="shared" si="10"/>
         <v>265.95</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="9">
         <f t="shared" si="10"/>
         <v>503.8</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="9">
         <f t="shared" si="10"/>
         <v>943.85</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="9">
         <f t="shared" si="10"/>
         <v>2418.4499999999998</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="9">
         <f t="shared" si="10"/>
         <v>4833.8999999999996</v>
       </c>
-      <c r="I95">
+      <c r="I95" s="9">
         <f t="shared" si="10"/>
         <v>18785.150000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+      <c r="B97">
+        <f>B68+B45</f>
+        <v>2.7617909316522309</v>
+      </c>
+      <c r="C97">
+        <f t="shared" ref="C97:L97" si="11">C68+C45</f>
+        <v>8.0095410939322136</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="11"/>
+        <v>4.5821242374461786</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="11"/>
+        <v>4.1073491058415499</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="11"/>
+        <v>6.9328761053956818</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="11"/>
+        <v>7.3892484185925582</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="11"/>
+        <v>9.1466679931468828</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="11"/>
+        <v>17.573380843125719</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="11"/>
+        <v>40.779495434196264</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="11"/>
+        <v>49.265586421202158</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="11"/>
+        <v>127.91657193279842</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98">
+        <f>B91+B68+B45</f>
+        <v>3.648832139975247</v>
+      </c>
+      <c r="C98">
+        <f t="shared" ref="C98:I98" si="12">C91+C68+C45</f>
+        <v>11.910957840651147</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="12"/>
+        <v>10.680225753923512</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="12"/>
+        <v>30.191978578710092</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="12"/>
+        <v>112.59997998406372</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="12"/>
+        <v>160.69540924511782</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="12"/>
+        <v>336.26548995882121</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="12"/>
+        <v>1326.048668705823</v>
       </c>
     </row>
   </sheetData>
@@ -11851,1107 +13689,462 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22423169-F610-5D44-A197-3E9349A36209}">
-  <dimension ref="O10:AC20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D6017C-F992-9741-B3D4-9EFFFE4BEDC6}">
+  <dimension ref="A3:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10:AC20"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S10" t="s">
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="T10" t="s">
-        <v>29</v>
-      </c>
-      <c r="U10" t="s">
-        <v>30</v>
-      </c>
-      <c r="V10" t="s">
-        <v>31</v>
-      </c>
-      <c r="W10" t="s">
-        <v>32</v>
-      </c>
-      <c r="X10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11">
-        <v>60</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>20</v>
-      </c>
-      <c r="R11">
-        <v>4</v>
-      </c>
-      <c r="S11">
-        <v>130</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11" t="s">
-        <v>41</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11">
-        <v>130</v>
-      </c>
-      <c r="X11" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z11">
-        <v>3</v>
-      </c>
-      <c r="AA11">
-        <v>1</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O12" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12">
-        <v>51</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R12">
-        <v>4</v>
-      </c>
-      <c r="S12">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.01</v>
+      </c>
+      <c r="B4">
+        <v>311</v>
+      </c>
+      <c r="C4">
+        <v>183</v>
+      </c>
+      <c r="D4">
+        <f>59+65</f>
+        <v>124</v>
+      </c>
+      <c r="E4">
+        <v>373</v>
+      </c>
+      <c r="F4">
+        <v>265</v>
+      </c>
+      <c r="G4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>311</v>
+      </c>
+      <c r="C5">
+        <v>183</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D14" si="0">59+65</f>
+        <v>124</v>
+      </c>
+      <c r="E5">
+        <v>373</v>
+      </c>
+      <c r="F5">
+        <v>265</v>
+      </c>
+      <c r="G5">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>311</v>
+      </c>
+      <c r="C6">
+        <v>183</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E6">
+        <v>373</v>
+      </c>
+      <c r="F6">
+        <v>263</v>
+      </c>
+      <c r="G6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>311</v>
+      </c>
+      <c r="C7">
+        <v>183</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E7">
+        <v>361</v>
+      </c>
+      <c r="F7">
+        <v>243</v>
+      </c>
+      <c r="G7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>311</v>
+      </c>
+      <c r="C8">
+        <v>183</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E8">
+        <v>361</v>
+      </c>
+      <c r="F8">
+        <v>240</v>
+      </c>
+      <c r="G8">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>311</v>
+      </c>
+      <c r="C9">
+        <v>183</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E9">
+        <v>352</v>
+      </c>
+      <c r="F9">
+        <v>228</v>
+      </c>
+      <c r="G9">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>311</v>
+      </c>
+      <c r="C10">
+        <v>183</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E10">
+        <v>334</v>
+      </c>
+      <c r="F10">
+        <v>206</v>
+      </c>
+      <c r="G10">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>311</v>
+      </c>
+      <c r="C11">
+        <v>183</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E11">
+        <v>326</v>
+      </c>
+      <c r="F11">
+        <v>182</v>
+      </c>
+      <c r="G11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>311</v>
+      </c>
+      <c r="C12">
+        <v>183</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E12">
+        <v>326</v>
+      </c>
+      <c r="F12">
+        <v>173</v>
+      </c>
+      <c r="G12">
         <v>110</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12" t="s">
-        <v>41</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.9</v>
+      </c>
+      <c r="B13">
+        <v>311</v>
+      </c>
+      <c r="C13">
+        <v>183</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E13">
+        <v>311</v>
+      </c>
+      <c r="F13">
+        <v>154</v>
+      </c>
+      <c r="G13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>311</v>
+      </c>
+      <c r="C14">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E14">
+        <v>311</v>
+      </c>
+      <c r="F14">
+        <v>139</v>
+      </c>
+      <c r="G14">
         <v>92</v>
       </c>
-      <c r="X12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z12">
-        <v>2</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O13" t="s">
-        <v>46</v>
-      </c>
-      <c r="P13">
-        <v>67</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13">
-        <v>4</v>
-      </c>
-      <c r="S13">
-        <v>106</v>
-      </c>
-      <c r="T13">
-        <v>223</v>
-      </c>
-      <c r="U13" t="s">
-        <v>22</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>142</v>
-      </c>
-      <c r="X13" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z13">
-        <v>1</v>
-      </c>
-      <c r="AA13">
-        <v>2</v>
-      </c>
-      <c r="AB13">
-        <v>3</v>
-      </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O14" t="s">
-        <v>48</v>
-      </c>
-      <c r="P14">
-        <v>35</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>22</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>120</v>
-      </c>
-      <c r="T14">
-        <v>160</v>
-      </c>
-      <c r="U14" t="s">
-        <v>22</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14">
-        <v>185</v>
-      </c>
-      <c r="X14" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O15" t="s">
-        <v>50</v>
-      </c>
-      <c r="P15">
-        <v>55</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>20</v>
-      </c>
-      <c r="R15">
-        <v>4</v>
-      </c>
-      <c r="S15">
-        <v>150</v>
-      </c>
-      <c r="T15">
-        <v>160</v>
-      </c>
-      <c r="U15" t="s">
-        <v>22</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>150</v>
-      </c>
-      <c r="X15" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O16" t="s">
-        <v>46</v>
-      </c>
-      <c r="P16">
-        <v>56</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>20</v>
-      </c>
-      <c r="R16">
-        <v>3</v>
-      </c>
-      <c r="S16">
-        <v>130</v>
-      </c>
-      <c r="T16">
-        <v>256</v>
-      </c>
-      <c r="U16" t="s">
-        <v>20</v>
-      </c>
-      <c r="V16">
-        <v>2</v>
-      </c>
-      <c r="W16">
-        <v>142</v>
-      </c>
-      <c r="X16" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z16">
-        <v>2</v>
-      </c>
-      <c r="AA16">
-        <v>1</v>
-      </c>
-      <c r="AB16">
-        <v>6</v>
-      </c>
-      <c r="AC16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O17" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17">
-        <v>51</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R17">
-        <v>4</v>
-      </c>
-      <c r="S17">
-        <v>95</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17" t="s">
-        <v>41</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>126</v>
-      </c>
-      <c r="X17" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z17">
-        <v>2</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O18" t="s">
-        <v>48</v>
-      </c>
-      <c r="P18">
-        <v>46</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>20</v>
-      </c>
-      <c r="R18">
-        <v>4</v>
-      </c>
-      <c r="S18">
-        <v>118</v>
-      </c>
-      <c r="T18">
-        <v>186</v>
-      </c>
-      <c r="U18" t="s">
-        <v>22</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>124</v>
-      </c>
-      <c r="X18" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB18">
-        <v>7</v>
-      </c>
-      <c r="AC18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O19" t="s">
-        <v>46</v>
-      </c>
-      <c r="P19">
-        <v>65</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>22</v>
-      </c>
-      <c r="R19">
-        <v>4</v>
-      </c>
-      <c r="S19">
-        <v>150</v>
-      </c>
-      <c r="T19">
-        <v>225</v>
-      </c>
-      <c r="U19" t="s">
-        <v>22</v>
-      </c>
-      <c r="V19">
-        <v>2</v>
-      </c>
-      <c r="W19">
-        <v>114</v>
-      </c>
-      <c r="X19" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z19">
-        <v>2</v>
-      </c>
-      <c r="AA19">
-        <v>3</v>
-      </c>
-      <c r="AB19">
-        <v>7</v>
-      </c>
-      <c r="AC19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="15:29" x14ac:dyDescent="0.2">
-      <c r="O20" t="s">
-        <v>48</v>
-      </c>
-      <c r="P20">
-        <v>50</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R20">
-        <v>4</v>
-      </c>
-      <c r="S20">
-        <v>145</v>
-      </c>
-      <c r="T20">
-        <v>264</v>
-      </c>
-      <c r="U20" t="s">
-        <v>22</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>150</v>
-      </c>
-      <c r="X20" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC20">
-        <v>1</v>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" ref="E16:F16" si="1">E4/B4</f>
+        <v>1.1993569131832797</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>1.4480874316939891</v>
+      </c>
+      <c r="G16">
+        <f>G4/D4</f>
+        <v>1.5887096774193548</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f t="shared" ref="E17:E29" si="2">E5/B5</f>
+        <v>1.1993569131832797</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:G29" si="3">F5/C5</f>
+        <v>1.4480874316939891</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1.5887096774193548</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1.1993569131832797</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>1.4371584699453552</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G29" si="4">G6/D6</f>
+        <v>1.4516129032258065</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1.1607717041800643</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>1.3278688524590163</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>1.4516129032258065</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1.1607717041800643</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>1.3114754098360655</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>1.4193548387096775</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1.1318327974276527</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>1.2459016393442623</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>1.1774193548387097</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1.0739549839228295</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>1.1256830601092895</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>1.1774193548387097</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>1.0482315112540193</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0.99453551912568305</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>1.0241935483870968</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>1.0482315112540193</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>0.94535519125683065</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>0.88709677419354838</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>0.84153005464480879</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>0.83870967741935487</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>0.7595628415300546</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>0.74193548387096775</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D14BEF-BBB9-6443-981F-D40A2FE47238}">
-  <dimension ref="A1:O11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>130</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>130</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>110</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>92</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>106</v>
-      </c>
-      <c r="F4">
-        <v>223</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>120</v>
-      </c>
-      <c r="F5">
-        <v>160</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>185</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" t="s">
-        <v>43</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>150</v>
-      </c>
-      <c r="F6">
-        <v>160</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>150</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>130</v>
-      </c>
-      <c r="F7">
-        <v>256</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>142</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>6</v>
-      </c>
-      <c r="O7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>95</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>126</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>118</v>
-      </c>
-      <c r="F9">
-        <v>186</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>124</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9">
-        <v>7</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>150</v>
-      </c>
-      <c r="F10">
-        <v>225</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>114</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10">
-        <v>2</v>
-      </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10">
-        <v>7</v>
-      </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>145</v>
-      </c>
-      <c r="F11">
-        <v>264</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>150</v>
-      </c>
-      <c r="J11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11" t="s">
-        <v>49</v>
-      </c>
-      <c r="M11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N11" t="s">
-        <v>43</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>